<commit_message>
automation test script has been added
</commit_message>
<xml_diff>
--- a/Manual Testing Project/OpenCart/OpenCart-TestCases.xlsx
+++ b/Manual Testing Project/OpenCart/OpenCart-TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120" tabRatio="914" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9120" tabRatio="914" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="2" r:id="rId1"/>
@@ -875,7 +875,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Email Address - pavanoltraining@gmail.com
+    <t xml:space="preserve">Email Address - rachitmore2@gmail.com
 Password -
 12345
 </t>
@@ -940,7 +940,7 @@
 5. Click on 'Login' button (Validate ER-1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Email Address - pavanoltraining@gmail.com
+    <t xml:space="preserve">Email Address - rachitmore2@gmail.com
 Password -
 xyzabc123
 </t>
@@ -15017,7 +15017,7 @@
   <sheetPr/>
   <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
@@ -20370,7 +20370,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="E10" workbookViewId="0">
+    <sheetView zoomScale="61" zoomScaleNormal="61" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -23035,8 +23035,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="64" zoomScaleNormal="64" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
@@ -24945,7 +24945,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -25644,7 +25644,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>